<commit_message>
- Map improvements - Fig for cluster cutoff - Summary table for alternative metrics
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -12,12 +12,13 @@
     <sheet name="trend_table_n_clicks" r:id="rId6" sheetId="4"/>
     <sheet name="trend_table_n_encounters" r:id="rId7" sheetId="5"/>
     <sheet name="trend_table_n_trains" r:id="rId8" sheetId="6"/>
+    <sheet name="trend_summary" r:id="rId9" sheetId="7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>station</t>
   </si>
@@ -305,6 +306,21 @@
   </si>
   <si>
     <t>0.52 (0.14)</t>
+  </si>
+  <si>
+    <t>dph</t>
+  </si>
+  <si>
+    <t>dps</t>
+  </si>
+  <si>
+    <t>n_clicks</t>
+  </si>
+  <si>
+    <t>n_encounters</t>
+  </si>
+  <si>
+    <t>n_trains</t>
   </si>
 </sst>
 </file>
@@ -1686,4 +1702,130 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>